<commit_message>
feat: Add SVG support and update image paths for belichtungspaket overlays
- Introduced SVG format support in the image API route for enhanced image versatility.
- Updated belichtungspaket overlay image paths to reflect new naming conventions for consistency across the application.
</commit_message>
<xml_diff>
--- a/preiskalkulation/Preiskalkulation_neu.xlsx
+++ b/preiskalkulation/Preiskalkulation_neu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jst01\source\repos\nest-haus\preiskalkulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A3DEF87-CF64-44AB-B574-FD491121246B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F55D027-4EC0-4215-8E78-0A9A6423CD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-9870" windowWidth="38620" windowHeight="21100" xr2:uid="{5CC58F37-0128-450E-8081-AE5F2D4C7F31}"/>
+    <workbookView xWindow="19110" yWindow="-9760" windowWidth="19380" windowHeight="20970" xr2:uid="{5CC58F37-0128-450E-8081-AE5F2D4C7F31}"/>
   </bookViews>
   <sheets>
     <sheet name="Preiskalkulation Zarnhofer" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="221">
   <si>
     <t>Preiskalkulation</t>
   </si>
@@ -688,6 +688,15 @@
   </si>
   <si>
     <t>pro m²</t>
+  </si>
+  <si>
+    <t>Geschossdecke Parkett</t>
+  </si>
+  <si>
+    <t>altes xsl: 2192,48</t>
+  </si>
+  <si>
+    <t>Parkett Eiche</t>
   </si>
 </sst>
 </file>
@@ -915,8 +924,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2BFBD1B5-50FA-4F58-8A9A-4701B499671D}" name="Tabelle1" displayName="Tabelle1" ref="A1:M80" totalsRowShown="0">
-  <autoFilter ref="A1:M80" xr:uid="{2BFBD1B5-50FA-4F58-8A9A-4701B499671D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2BFBD1B5-50FA-4F58-8A9A-4701B499671D}" name="Tabelle1" displayName="Tabelle1" ref="A1:M82" totalsRowShown="0">
+  <autoFilter ref="A1:M82" xr:uid="{2BFBD1B5-50FA-4F58-8A9A-4701B499671D}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{804CA334-FA10-447C-A09B-A78991FCA8B6}" name="Preiskalkulation" dataDxfId="25"/>
     <tableColumn id="2" xr3:uid="{D4477554-84AA-466D-BE89-525FCD624D3D}" name="Beschreibung" dataDxfId="24"/>
@@ -937,8 +946,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{311A614D-A764-48AB-BBEB-F7AA9FE00D10}" name="Tabelle2" displayName="Tabelle2" ref="A82:L118" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="A82:L118" xr:uid="{311A614D-A764-48AB-BBEB-F7AA9FE00D10}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{311A614D-A764-48AB-BBEB-F7AA9FE00D10}" name="Tabelle2" displayName="Tabelle2" ref="A84:L120" totalsRowShown="0" headerRowDxfId="15">
+  <autoFilter ref="A84:L120" xr:uid="{311A614D-A764-48AB-BBEB-F7AA9FE00D10}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{33BB18F3-BF03-4681-BBBC-6815896D3F7A}" name="Gebäudehülle" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{9CA0B145-8116-454B-B6EE-F6B17BEE6EFB}" name="Kombination Hülle, Innenv., Bodenb." dataDxfId="16"/>
@@ -1274,10 +1283,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7E85103-D0D9-40AB-A29F-2FB7E288D9F5}">
-  <dimension ref="A1:P118"/>
+  <dimension ref="A1:P120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R102" sqref="R101:R102"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1964,92 +1973,92 @@
       <c r="M32" s="2"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" s="13">
-        <v>102.35</v>
-      </c>
-      <c r="D33" s="13">
-        <v>20.5288</v>
-      </c>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13">
-        <f>C33*D33</f>
-        <v>2101.1226799999999</v>
-      </c>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="L33" s="12"/>
-      <c r="M33" s="12"/>
+      <c r="B33" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C33" s="4">
+        <v>106.8</v>
+      </c>
+      <c r="D33" s="4">
+        <v>20.53</v>
+      </c>
+      <c r="F33" s="4">
+        <f>Tabelle1[[#This Row],[Einzelpreis m²]]*Tabelle1[[#This Row],[m²/Modul]]</f>
+        <v>2192.6040000000003</v>
+      </c>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>195</v>
+        <v>62</v>
       </c>
       <c r="C34" s="13">
-        <v>127.3</v>
+        <v>102.35</v>
       </c>
       <c r="D34" s="13">
-        <v>20.53</v>
+        <v>20.5288</v>
       </c>
       <c r="E34" s="13"/>
       <c r="F34" s="13">
         <f>C34*D34</f>
-        <v>2613.4690000000001</v>
+        <v>2101.1226799999999</v>
       </c>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
       <c r="I34" s="13"/>
       <c r="J34" s="13"/>
-      <c r="K34" s="12"/>
+      <c r="K34" s="12" t="s">
+        <v>196</v>
+      </c>
       <c r="L34" s="12"/>
       <c r="M34" s="12"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A35" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10">
-        <v>141.9</v>
-      </c>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
+      <c r="A35" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="C35" s="13">
+        <v>127.3</v>
+      </c>
+      <c r="D35" s="13">
+        <v>20.53</v>
+      </c>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13">
+        <f>C35*D35</f>
+        <v>2613.4690000000001</v>
+      </c>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10">
-        <v>2307.64</v>
+        <v>141.9</v>
       </c>
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
@@ -2060,119 +2069,122 @@
       <c r="M36" s="9"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10">
+        <v>2307.64</v>
+      </c>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="21"/>
+      <c r="B38" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="C38" s="22">
+        <v>106.8</v>
+      </c>
+      <c r="D38" s="22">
+        <v>20.53</v>
+      </c>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22">
+        <f>Tabelle1[[#This Row],[Einzelpreis m²]]*Tabelle1[[#This Row],[m²/Modul]]</f>
+        <v>2192.6040000000003</v>
+      </c>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="L38" s="22"/>
+      <c r="M38" s="22"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B39" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15">
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15">
         <v>155.44999999999999</v>
       </c>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B40" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E40" s="6">
         <v>1614.35</v>
       </c>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="2" t="s">
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B41" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E41" s="6">
         <v>225</v>
       </c>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="2" t="s">
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A40" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19">
-        <v>1423.39</v>
-      </c>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="18"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A41" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B41" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19">
-        <v>2060</v>
-      </c>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C42" s="19"/>
       <c r="D42" s="19"/>
       <c r="E42" s="19">
-        <v>2430.08</v>
+        <v>1423.39</v>
       </c>
       <c r="F42" s="19"/>
       <c r="G42" s="19"/>
@@ -2185,18 +2197,20 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C43" s="19"/>
       <c r="D43" s="19"/>
       <c r="E43" s="19">
-        <v>6914.38</v>
+        <v>2060</v>
       </c>
       <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
+      <c r="G43" s="19" t="s">
+        <v>77</v>
+      </c>
       <c r="H43" s="19"/>
       <c r="I43" s="19"/>
       <c r="J43" s="19"/>
@@ -2206,15 +2220,15 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="C44" s="19"/>
       <c r="D44" s="19"/>
       <c r="E44" s="19">
-        <v>2751.63</v>
+        <v>2430.08</v>
       </c>
       <c r="F44" s="19"/>
       <c r="G44" s="19"/>
@@ -2227,15 +2241,15 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C45" s="19"/>
       <c r="D45" s="19"/>
       <c r="E45" s="19">
-        <v>4246.6000000000004</v>
+        <v>6914.38</v>
       </c>
       <c r="F45" s="19"/>
       <c r="G45" s="19"/>
@@ -2248,15 +2262,15 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
       <c r="E46" s="19">
-        <v>1083.07</v>
+        <v>2751.63</v>
       </c>
       <c r="F46" s="19"/>
       <c r="G46" s="19"/>
@@ -2269,15 +2283,15 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="18" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C47" s="19"/>
       <c r="D47" s="19"/>
       <c r="E47" s="19">
-        <v>1454.5</v>
+        <v>4246.6000000000004</v>
       </c>
       <c r="F47" s="19"/>
       <c r="G47" s="19"/>
@@ -2290,15 +2304,15 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="18" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C48" s="19"/>
       <c r="D48" s="19"/>
       <c r="E48" s="19">
-        <v>2159.2600000000002</v>
+        <v>1083.07</v>
       </c>
       <c r="F48" s="19"/>
       <c r="G48" s="19"/>
@@ -2311,15 +2325,15 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="18" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="C49" s="19"/>
       <c r="D49" s="19"/>
       <c r="E49" s="19">
-        <v>6141.59</v>
+        <v>1454.5</v>
       </c>
       <c r="F49" s="19"/>
       <c r="G49" s="19"/>
@@ -2332,15 +2346,15 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C50" s="19"/>
       <c r="D50" s="19"/>
       <c r="E50" s="19">
-        <v>1873.07</v>
+        <v>2159.2600000000002</v>
       </c>
       <c r="F50" s="19"/>
       <c r="G50" s="19"/>
@@ -2353,15 +2367,15 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="18" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="C51" s="19"/>
       <c r="D51" s="19"/>
       <c r="E51" s="19">
-        <v>4246.6000000000004</v>
+        <v>6141.59</v>
       </c>
       <c r="F51" s="19"/>
       <c r="G51" s="19"/>
@@ -2374,16 +2388,16 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="18" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="C52" s="19">
-        <v>1228.55</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="C52" s="19"/>
       <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
+      <c r="E52" s="19">
+        <v>1873.07</v>
+      </c>
       <c r="F52" s="19"/>
       <c r="G52" s="19"/>
       <c r="H52" s="19"/>
@@ -2395,16 +2409,16 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="18" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="C53" s="19">
-        <v>1539.05</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="C53" s="19"/>
       <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
+      <c r="E53" s="19">
+        <v>4246.6000000000004</v>
+      </c>
       <c r="F53" s="19"/>
       <c r="G53" s="19"/>
       <c r="H53" s="19"/>
@@ -2416,13 +2430,13 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C54" s="19">
-        <v>1925.45</v>
+        <v>1228.55</v>
       </c>
       <c r="D54" s="19"/>
       <c r="E54" s="19"/>
@@ -2437,13 +2451,13 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C55" s="19">
-        <v>1050.3</v>
+        <v>1539.05</v>
       </c>
       <c r="D55" s="19"/>
       <c r="E55" s="19"/>
@@ -2458,16 +2472,16 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="18" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="C56" s="19"/>
+        <v>105</v>
+      </c>
+      <c r="C56" s="19">
+        <v>1925.45</v>
+      </c>
       <c r="D56" s="19"/>
-      <c r="E56" s="19">
-        <v>3930.48</v>
-      </c>
+      <c r="E56" s="19"/>
       <c r="F56" s="19"/>
       <c r="G56" s="19"/>
       <c r="H56" s="19"/>
@@ -2479,16 +2493,16 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="18" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="C57" s="19"/>
+        <v>106</v>
+      </c>
+      <c r="C57" s="19">
+        <v>1050.3</v>
+      </c>
       <c r="D57" s="19"/>
-      <c r="E57" s="19">
-        <v>7258</v>
-      </c>
+      <c r="E57" s="19"/>
       <c r="F57" s="19"/>
       <c r="G57" s="19"/>
       <c r="H57" s="19"/>
@@ -2500,15 +2514,15 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="18" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C58" s="19"/>
       <c r="D58" s="19"/>
       <c r="E58" s="19">
-        <v>4838.3999999999996</v>
+        <v>3930.48</v>
       </c>
       <c r="F58" s="19"/>
       <c r="G58" s="19"/>
@@ -2521,16 +2535,16 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="18" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="C59" s="19">
-        <v>1295.25</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="C59" s="19"/>
       <c r="D59" s="19"/>
-      <c r="E59" s="19"/>
+      <c r="E59" s="19">
+        <v>7258</v>
+      </c>
       <c r="F59" s="19"/>
       <c r="G59" s="19"/>
       <c r="H59" s="19"/>
@@ -2542,16 +2556,16 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="C60" s="19">
-        <v>1637.95</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="C60" s="19"/>
       <c r="D60" s="19"/>
-      <c r="E60" s="19"/>
+      <c r="E60" s="19">
+        <v>4838.3999999999996</v>
+      </c>
       <c r="F60" s="19"/>
       <c r="G60" s="19"/>
       <c r="H60" s="19"/>
@@ -2563,13 +2577,13 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C61" s="19">
-        <v>2055.98</v>
+        <v>1295.25</v>
       </c>
       <c r="D61" s="19"/>
       <c r="E61" s="19"/>
@@ -2584,13 +2598,13 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="18" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C62" s="19">
-        <v>1094</v>
+        <v>1637.95</v>
       </c>
       <c r="D62" s="19"/>
       <c r="E62" s="19"/>
@@ -2605,16 +2619,16 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="18" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B63" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="C63" s="19"/>
+        <v>119</v>
+      </c>
+      <c r="C63" s="19">
+        <v>2055.98</v>
+      </c>
       <c r="D63" s="19"/>
-      <c r="E63" s="19">
-        <v>3930.48</v>
-      </c>
+      <c r="E63" s="19"/>
       <c r="F63" s="19"/>
       <c r="G63" s="19"/>
       <c r="H63" s="19"/>
@@ -2626,16 +2640,16 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="18" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="C64" s="19"/>
+        <v>120</v>
+      </c>
+      <c r="C64" s="19">
+        <v>1094</v>
+      </c>
       <c r="D64" s="19"/>
-      <c r="E64" s="19">
-        <v>7893.95</v>
-      </c>
+      <c r="E64" s="19"/>
       <c r="F64" s="19"/>
       <c r="G64" s="19"/>
       <c r="H64" s="19"/>
@@ -2647,15 +2661,15 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="18" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C65" s="19"/>
       <c r="D65" s="19"/>
       <c r="E65" s="19">
-        <v>5309.9</v>
+        <v>3930.48</v>
       </c>
       <c r="F65" s="19"/>
       <c r="G65" s="19"/>
@@ -2668,16 +2682,16 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="18" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="C66" s="19">
-        <v>921.5</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="C66" s="19"/>
       <c r="D66" s="19"/>
-      <c r="E66" s="19"/>
+      <c r="E66" s="19">
+        <v>7893.95</v>
+      </c>
       <c r="F66" s="19"/>
       <c r="G66" s="19"/>
       <c r="H66" s="19"/>
@@ -2689,16 +2703,16 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="18" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="C67" s="19">
-        <v>1034.2</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="C67" s="19"/>
       <c r="D67" s="19"/>
-      <c r="E67" s="19"/>
+      <c r="E67" s="19">
+        <v>5309.9</v>
+      </c>
       <c r="F67" s="19"/>
       <c r="G67" s="19"/>
       <c r="H67" s="19"/>
@@ -2710,13 +2724,13 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C68" s="19">
-        <v>1101.48</v>
+        <v>921.5</v>
       </c>
       <c r="D68" s="19"/>
       <c r="E68" s="19"/>
@@ -2731,13 +2745,13 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C69" s="19">
-        <v>881.25</v>
+        <v>1034.2</v>
       </c>
       <c r="D69" s="19"/>
       <c r="E69" s="19"/>
@@ -2752,16 +2766,16 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="C70" s="19"/>
+        <v>136</v>
+      </c>
+      <c r="C70" s="19">
+        <v>1101.48</v>
+      </c>
       <c r="D70" s="19"/>
-      <c r="E70" s="19">
-        <v>3663.67</v>
-      </c>
+      <c r="E70" s="19"/>
       <c r="F70" s="19"/>
       <c r="G70" s="19"/>
       <c r="H70" s="19"/>
@@ -2773,16 +2787,16 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="C71" s="19"/>
+        <v>137</v>
+      </c>
+      <c r="C71" s="19">
+        <v>881.25</v>
+      </c>
       <c r="D71" s="19"/>
-      <c r="E71" s="19">
-        <v>5071.8500000000004</v>
-      </c>
+      <c r="E71" s="19"/>
       <c r="F71" s="19"/>
       <c r="G71" s="19"/>
       <c r="H71" s="19"/>
@@ -2794,15 +2808,15 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C72" s="19"/>
       <c r="D72" s="19"/>
       <c r="E72" s="19">
-        <v>3483.7</v>
+        <v>3663.67</v>
       </c>
       <c r="F72" s="19"/>
       <c r="G72" s="19"/>
@@ -2814,119 +2828,125 @@
       <c r="M72" s="18"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A73" s="14" t="s">
+      <c r="A73" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="B73" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="C73" s="19"/>
+      <c r="D73" s="19"/>
+      <c r="E73" s="19">
+        <v>5071.8500000000004</v>
+      </c>
+      <c r="F73" s="19"/>
+      <c r="G73" s="19"/>
+      <c r="H73" s="19"/>
+      <c r="I73" s="19"/>
+      <c r="J73" s="19"/>
+      <c r="K73" s="18"/>
+      <c r="L73" s="18"/>
+      <c r="M73" s="18"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A74" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B74" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="C74" s="19"/>
+      <c r="D74" s="19"/>
+      <c r="E74" s="19">
+        <v>3483.7</v>
+      </c>
+      <c r="F74" s="19"/>
+      <c r="G74" s="19"/>
+      <c r="H74" s="19"/>
+      <c r="I74" s="19"/>
+      <c r="J74" s="19"/>
+      <c r="K74" s="18"/>
+      <c r="L74" s="18"/>
+      <c r="M74" s="18"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A75" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="B73" s="14" t="s">
+      <c r="B75" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="C73" s="15"/>
-      <c r="D73" s="15"/>
-      <c r="E73" s="15">
+      <c r="C75" s="15"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="15">
         <v>2971.5</v>
       </c>
-      <c r="F73" s="15"/>
-      <c r="G73" s="15"/>
-      <c r="H73" s="15"/>
-      <c r="I73" s="15"/>
-      <c r="J73" s="15"/>
-      <c r="K73" s="14" t="s">
+      <c r="F75" s="15"/>
+      <c r="G75" s="15"/>
+      <c r="H75" s="15"/>
+      <c r="I75" s="15"/>
+      <c r="J75" s="15"/>
+      <c r="K75" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="L73" s="14"/>
-      <c r="M73" s="14"/>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A74" s="14" t="s">
+      <c r="L75" s="14"/>
+      <c r="M75" s="14"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A76" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="B74" s="14" t="s">
+      <c r="B76" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="C74" s="15"/>
-      <c r="D74" s="15"/>
-      <c r="E74" s="15">
+      <c r="C76" s="15"/>
+      <c r="D76" s="15"/>
+      <c r="E76" s="15">
         <v>1408.75</v>
       </c>
-      <c r="F74" s="15"/>
-      <c r="G74" s="15"/>
-      <c r="H74" s="15"/>
-      <c r="I74" s="15"/>
-      <c r="J74" s="15"/>
-      <c r="K74" s="14" t="s">
+      <c r="F76" s="15"/>
+      <c r="G76" s="15"/>
+      <c r="H76" s="15"/>
+      <c r="I76" s="15"/>
+      <c r="J76" s="15"/>
+      <c r="K76" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="L74" s="14"/>
-      <c r="M74" s="14"/>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A75" s="16" t="s">
+      <c r="L76" s="14"/>
+      <c r="M76" s="14"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A77" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="B75" s="16" t="s">
+      <c r="B77" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="C75" s="17"/>
-      <c r="D75" s="17"/>
-      <c r="E75" s="17"/>
-      <c r="F75" s="17">
+      <c r="C77" s="17"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="17">
         <v>3000</v>
       </c>
-      <c r="G75" s="17"/>
-      <c r="H75" s="17"/>
-      <c r="I75" s="17"/>
-      <c r="J75" s="17"/>
-      <c r="K75" s="16"/>
-      <c r="L75" s="16"/>
-      <c r="M75" s="16"/>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A76" s="21" t="s">
+      <c r="G77" s="17"/>
+      <c r="H77" s="17"/>
+      <c r="I77" s="17"/>
+      <c r="J77" s="17"/>
+      <c r="K77" s="16"/>
+      <c r="L77" s="16"/>
+      <c r="M77" s="16"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A78" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B76" s="21" t="s">
+      <c r="B78" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="C76" s="22"/>
-      <c r="D76" s="22">
+      <c r="C78" s="22"/>
+      <c r="D78" s="22">
         <v>20.53</v>
       </c>
-      <c r="E76" s="22"/>
-      <c r="F76" s="22"/>
-      <c r="G76" s="22"/>
-      <c r="H76" s="22"/>
-      <c r="I76" s="22"/>
-      <c r="J76" s="22"/>
-      <c r="K76" s="21"/>
-      <c r="L76" s="22"/>
-      <c r="M76" s="22"/>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A77" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="B77" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="C77" s="22"/>
-      <c r="D77" s="22">
-        <v>20.53</v>
-      </c>
-      <c r="E77" s="22"/>
-      <c r="F77" s="22"/>
-      <c r="G77" s="22"/>
-      <c r="H77" s="22"/>
-      <c r="I77" s="22"/>
-      <c r="J77" s="22"/>
-      <c r="K77" s="21"/>
-      <c r="L77" s="22"/>
-      <c r="M77" s="22"/>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A78" s="21"/>
-      <c r="B78" s="21"/>
-      <c r="C78" s="22"/>
-      <c r="D78" s="22"/>
       <c r="E78" s="22"/>
       <c r="F78" s="22"/>
       <c r="G78" s="22"/>
@@ -2938,10 +2958,16 @@
       <c r="M78" s="22"/>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A79" s="21"/>
-      <c r="B79" s="21"/>
+      <c r="A79" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="B79" s="21" t="s">
+        <v>210</v>
+      </c>
       <c r="C79" s="22"/>
-      <c r="D79" s="22"/>
+      <c r="D79" s="22">
+        <v>20.53</v>
+      </c>
       <c r="E79" s="22"/>
       <c r="F79" s="22"/>
       <c r="G79" s="22"/>
@@ -2953,177 +2979,111 @@
       <c r="M79" s="22"/>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="H80" s="4"/>
-      <c r="I80" s="4"/>
-      <c r="J80" s="4"/>
-      <c r="K80" s="2"/>
-      <c r="L80" s="4"/>
-      <c r="M80" s="4"/>
+      <c r="A80" s="21"/>
+      <c r="B80" s="21"/>
+      <c r="C80" s="22"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="22"/>
+      <c r="F80" s="22"/>
+      <c r="G80" s="22"/>
+      <c r="H80" s="22"/>
+      <c r="I80" s="22"/>
+      <c r="J80" s="22"/>
+      <c r="K80" s="21"/>
+      <c r="L80" s="22"/>
+      <c r="M80" s="22"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="P81" t="s">
+      <c r="A81" s="21"/>
+      <c r="B81" s="21"/>
+      <c r="C81" s="22"/>
+      <c r="D81" s="22"/>
+      <c r="E81" s="22"/>
+      <c r="F81" s="22"/>
+      <c r="G81" s="22"/>
+      <c r="H81" s="22"/>
+      <c r="I81" s="22"/>
+      <c r="J81" s="22"/>
+      <c r="K81" s="21"/>
+      <c r="L81" s="22"/>
+      <c r="M81" s="22"/>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H82" s="4"/>
+      <c r="I82" s="4"/>
+      <c r="J82" s="4"/>
+      <c r="K82" s="2"/>
+      <c r="L82" s="4"/>
+      <c r="M82" s="4"/>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P83" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A82" s="20" t="s">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A84" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C82" s="8" t="s">
+      <c r="C84" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="D82" s="8" t="s">
+      <c r="D84" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="E82" s="23" t="s">
+      <c r="E84" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="F82" s="4" t="s">
+      <c r="F84" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="G82" s="8" t="s">
+      <c r="G84" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="H82" s="4" t="s">
+      <c r="H84" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="I82" s="4" t="s">
+      <c r="I84" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="J82" s="4" t="s">
+      <c r="J84" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="K82" s="2" t="s">
+      <c r="K84" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="L82" s="4" t="s">
+      <c r="L84" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="N82" t="s">
+      <c r="N84" t="s">
         <v>214</v>
       </c>
-      <c r="O82">
-        <f>(4*F36)+(2*C83)+(2*D83)+(E83*4)+11*(C67*0.8)+F35</f>
+      <c r="O84">
+        <f>(4*F37)+(2*C85)+(2*D85)+(E85*4)+11*(C69*0.8)+F36</f>
         <v>150333.99059999999</v>
       </c>
-      <c r="P82">
-        <f>(2*C83)+(2*D83)+(E83*4)+11*(C67*0.8)+F35</f>
+      <c r="P84">
+        <f>(2*C85)+(2*D85)+(E85*4)+11*(C69*0.8)+F36</f>
         <v>141103.43059999999</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A83" s="2" t="s">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C83" s="4">
+      <c r="C85" s="4">
         <f>F6+F20</f>
         <v>23574.016</v>
       </c>
-      <c r="D83" s="4">
+      <c r="D85" s="4">
         <f>F10+F22</f>
         <v>36499.2693</v>
-      </c>
-      <c r="E83" s="4">
-        <f>F2</f>
-        <v>2928.5</v>
-      </c>
-      <c r="F83" s="4">
-        <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>12600.35706</v>
-      </c>
-      <c r="G83" s="4">
-        <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>6300.1785300000001</v>
-      </c>
-      <c r="H83" s="4">
-        <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>150761.10619000002</v>
-      </c>
-      <c r="I83" s="4">
-        <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>177263.62218999999</v>
-      </c>
-      <c r="J83" s="4">
-        <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>203766.13819</v>
-      </c>
-      <c r="K83" s="1">
-        <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>230268.65419</v>
-      </c>
-      <c r="L83">
-        <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>256771.17019</v>
-      </c>
-      <c r="N83" t="s">
-        <v>206</v>
-      </c>
-      <c r="O83">
-        <f>O82*0.2</f>
-        <v>30066.798119999999</v>
-      </c>
-      <c r="P83">
-        <f>P82*0.2</f>
-        <v>28220.686119999998</v>
-      </c>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B84" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E84" s="4">
-        <f t="shared" ref="E83:E118" si="0">F2</f>
-        <v>2928.5</v>
-      </c>
-      <c r="F84" s="4">
-        <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>585.70000000000005</v>
-      </c>
-      <c r="G84" s="4">
-        <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>292.85000000000002</v>
-      </c>
-      <c r="H84" s="4">
-        <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>12592.550000000001</v>
-      </c>
-      <c r="I84" s="4">
-        <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>15521.050000000001</v>
-      </c>
-      <c r="J84" s="4">
-        <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>18449.55</v>
-      </c>
-      <c r="K84" s="1">
-        <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>21378.05</v>
-      </c>
-      <c r="L84">
-        <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>24306.55</v>
-      </c>
-      <c r="N84" t="s">
-        <v>213</v>
-      </c>
-      <c r="O84">
-        <f>O82*0.1</f>
-        <v>15033.39906</v>
-      </c>
-      <c r="P84">
-        <f>P82*0.1</f>
-        <v>14110.343059999999</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B85" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="E85" s="4">
         <f>F2</f>
@@ -3131,47 +3091,55 @@
       </c>
       <c r="F85" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>585.70000000000005</v>
+        <v>12600.35706</v>
       </c>
       <c r="G85" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>292.85000000000002</v>
+        <v>6300.1785300000001</v>
       </c>
       <c r="H85" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>12592.550000000001</v>
+        <v>150761.10619000002</v>
       </c>
       <c r="I85" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>15521.050000000001</v>
+        <v>177263.62218999999</v>
       </c>
       <c r="J85" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>18449.55</v>
+        <v>203766.13819</v>
       </c>
       <c r="K85" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>21378.05</v>
+        <v>230268.65419</v>
       </c>
       <c r="L85">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>24306.55</v>
+        <v>256771.17019</v>
       </c>
       <c r="N85" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="O85">
-        <f>O82+O83+O84</f>
-        <v>195434.18777999998</v>
+        <f>O84*0.2</f>
+        <v>30066.798119999999</v>
       </c>
       <c r="P85">
-        <f>P82+P83+P84</f>
-        <v>183434.45977999998</v>
+        <f>P84*0.2</f>
+        <v>28220.686119999998</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B86" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
+      </c>
+      <c r="C86" s="4">
+        <f>F6+F20+F33</f>
+        <v>25766.62</v>
+      </c>
+      <c r="D86" s="4">
+        <f>F10+F22+F33</f>
+        <v>38691.873299999999</v>
       </c>
       <c r="E86" s="4">
         <f>F2</f>
@@ -3179,55 +3147,47 @@
       </c>
       <c r="F86" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>585.70000000000005</v>
+        <v>13477.398659999999</v>
       </c>
       <c r="G86" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>292.85000000000002</v>
+        <v>6738.6993299999995</v>
       </c>
       <c r="H86" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>12592.550000000001</v>
+        <v>160847.08459000001</v>
       </c>
       <c r="I86" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>15521.050000000001</v>
+        <v>189542.20459000001</v>
       </c>
       <c r="J86" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>18449.55</v>
+        <v>218237.32459</v>
       </c>
       <c r="K86" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>21378.05</v>
+        <v>246932.44459</v>
       </c>
       <c r="L86">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>24306.55</v>
+        <v>275627.56458999997</v>
       </c>
       <c r="N86" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="O86">
-        <f>O85/107</f>
-        <v>1826.4877362616821</v>
+        <f>O84*0.1</f>
+        <v>15033.39906</v>
       </c>
       <c r="P86">
-        <f>P85/75</f>
-        <v>2445.7927970666665</v>
+        <f>P84*0.1</f>
+        <v>14110.343059999999</v>
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B87" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C87" s="4">
-        <f>F6+F25</f>
-        <v>24808.461900000002</v>
-      </c>
-      <c r="D87" s="4">
-        <f>F10+F27</f>
-        <v>38714.5213</v>
+        <v>158</v>
       </c>
       <c r="E87" s="4">
         <f>F2</f>
@@ -3235,36 +3195,47 @@
       </c>
       <c r="F87" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>13290.29664</v>
+        <v>585.70000000000005</v>
       </c>
       <c r="G87" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>6645.1483200000002</v>
+        <v>292.85000000000002</v>
       </c>
       <c r="H87" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>158695.41136</v>
+        <v>12592.550000000001</v>
       </c>
       <c r="I87" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>186432.37326000005</v>
+        <v>15521.050000000001</v>
       </c>
       <c r="J87" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>214169.33516000005</v>
+        <v>18449.55</v>
       </c>
       <c r="K87" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>241906.29706000004</v>
+        <v>21378.05</v>
       </c>
       <c r="L87">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>269643.25896000001</v>
+        <v>24306.55</v>
+      </c>
+      <c r="N87" t="s">
+        <v>212</v>
+      </c>
+      <c r="O87">
+        <f>O84+O85+O86</f>
+        <v>195434.18777999998</v>
+      </c>
+      <c r="P87">
+        <f>P84+P85+P86</f>
+        <v>183434.45977999998</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B88" s="2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E88" s="4">
         <f>F2</f>
@@ -3298,10 +3269,29 @@
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
         <v>24306.55</v>
       </c>
+      <c r="N88" t="s">
+        <v>217</v>
+      </c>
+      <c r="O88">
+        <f>O87/107</f>
+        <v>1826.4877362616821</v>
+      </c>
+      <c r="P88">
+        <f>P87/75</f>
+        <v>2445.7927970666665</v>
+      </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B89" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
+      </c>
+      <c r="C89" s="4">
+        <f>F6+F25</f>
+        <v>24808.461900000002</v>
+      </c>
+      <c r="D89" s="4">
+        <f>F10+F27</f>
+        <v>38714.5213</v>
       </c>
       <c r="E89" s="4">
         <f>F2</f>
@@ -3309,36 +3299,44 @@
       </c>
       <c r="F89" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>585.70000000000005</v>
+        <v>13290.29664</v>
       </c>
       <c r="G89" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>292.85000000000002</v>
+        <v>6645.1483200000002</v>
       </c>
       <c r="H89" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>12592.550000000001</v>
+        <v>158695.41136</v>
       </c>
       <c r="I89" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>15521.050000000001</v>
+        <v>186432.37326000005</v>
       </c>
       <c r="J89" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>18449.55</v>
+        <v>214169.33516000005</v>
       </c>
       <c r="K89" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>21378.05</v>
+        <v>241906.29706000004</v>
       </c>
       <c r="L89">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>24306.55</v>
+        <v>269643.25896000001</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B90" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
+      </c>
+      <c r="C90" s="4">
+        <f>F6+F25+F33</f>
+        <v>27001.065900000001</v>
+      </c>
+      <c r="D90" s="4">
+        <f>F10+F27+F33</f>
+        <v>40907.1253</v>
       </c>
       <c r="E90" s="4">
         <f>F2</f>
@@ -3346,44 +3344,36 @@
       </c>
       <c r="F90" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>585.70000000000005</v>
+        <v>14167.338240000001</v>
       </c>
       <c r="G90" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>292.85000000000002</v>
+        <v>7083.6691200000005</v>
       </c>
       <c r="H90" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>12592.550000000001</v>
+        <v>168781.38976000002</v>
       </c>
       <c r="I90" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>15521.050000000001</v>
+        <v>198710.95566000001</v>
       </c>
       <c r="J90" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>18449.55</v>
+        <v>228640.52156000002</v>
       </c>
       <c r="K90" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>21378.05</v>
+        <v>258570.08746000001</v>
       </c>
       <c r="L90">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>24306.55</v>
+        <v>288499.65336</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B91" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C91" s="4">
-        <f>F6+F30</f>
-        <v>24104.409599999999</v>
-      </c>
-      <c r="D91" s="4">
-        <f>F10+F32</f>
-        <v>37451.077300000004</v>
+        <v>166</v>
       </c>
       <c r="E91" s="4">
         <f>F2</f>
@@ -3391,36 +3381,36 @@
       </c>
       <c r="F91" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>12896.797380000002</v>
+        <v>585.70000000000005</v>
       </c>
       <c r="G91" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>6448.3986900000009</v>
+        <v>292.85000000000002</v>
       </c>
       <c r="H91" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>154170.16987000001</v>
+        <v>12592.550000000001</v>
       </c>
       <c r="I91" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>181203.07947</v>
+        <v>15521.050000000001</v>
       </c>
       <c r="J91" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>208235.98907000001</v>
+        <v>18449.55</v>
       </c>
       <c r="K91" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>235268.89867000002</v>
+        <v>21378.05</v>
       </c>
       <c r="L91">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>262301.80826999998</v>
+        <v>24306.55</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B92" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E92" s="4">
         <f>F2</f>
@@ -3457,7 +3447,15 @@
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B93" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
+      </c>
+      <c r="C93" s="4">
+        <f>F6+F30</f>
+        <v>24104.409599999999</v>
+      </c>
+      <c r="D93" s="4">
+        <f>F10+F32</f>
+        <v>37451.077300000004</v>
       </c>
       <c r="E93" s="4">
         <f>F2</f>
@@ -3465,36 +3463,44 @@
       </c>
       <c r="F93" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>585.70000000000005</v>
+        <v>12896.797380000002</v>
       </c>
       <c r="G93" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>292.85000000000002</v>
+        <v>6448.3986900000009</v>
       </c>
       <c r="H93" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>12592.550000000001</v>
+        <v>154170.16987000001</v>
       </c>
       <c r="I93" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>15521.050000000001</v>
+        <v>181203.07947</v>
       </c>
       <c r="J93" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>18449.55</v>
+        <v>208235.98907000001</v>
       </c>
       <c r="K93" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>21378.05</v>
+        <v>235268.89867000002</v>
       </c>
       <c r="L93">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>24306.55</v>
+        <v>262301.80826999998</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B94" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
+      </c>
+      <c r="C94" s="4">
+        <f>F6+F30+F33</f>
+        <v>26297.013599999998</v>
+      </c>
+      <c r="D94" s="4">
+        <f>F6+F32+F33</f>
+        <v>28987.421300000002</v>
       </c>
       <c r="E94" s="4">
         <f>F2</f>
@@ -3502,47 +3508,36 @@
       </c>
       <c r="F94" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>585.70000000000005</v>
+        <v>11642.58698</v>
       </c>
       <c r="G94" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>292.85000000000002</v>
+        <v>5821.29349</v>
       </c>
       <c r="H94" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>12592.550000000001</v>
+        <v>139746.75027000002</v>
       </c>
       <c r="I94" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>15521.050000000001</v>
+        <v>168972.26387</v>
       </c>
       <c r="J94" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>18449.55</v>
+        <v>198197.77747</v>
       </c>
       <c r="K94" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>21378.05</v>
+        <v>227423.29107000001</v>
       </c>
       <c r="L94">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>24306.55</v>
+        <v>256648.80466999998</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A95" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="B95" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C95" s="4">
-        <f>F6+F20+F11</f>
-        <v>30101.097999999998</v>
-      </c>
-      <c r="D95" s="4">
-        <f>F10+F22+F12</f>
-        <v>48896.791299999997</v>
+        <v>170</v>
       </c>
       <c r="E95" s="4">
         <f>F2</f>
@@ -3550,36 +3545,36 @@
       </c>
       <c r="F95" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>16385.277859999998</v>
+        <v>585.70000000000005</v>
       </c>
       <c r="G95" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>8192.6389299999992</v>
+        <v>292.85000000000002</v>
       </c>
       <c r="H95" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>194287.69538999998</v>
+        <v>12592.550000000001</v>
       </c>
       <c r="I95" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>227317.29338999998</v>
+        <v>15521.050000000001</v>
       </c>
       <c r="J95" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>260346.89138999998</v>
+        <v>18449.55</v>
       </c>
       <c r="K95" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>293376.48938999994</v>
+        <v>21378.05</v>
       </c>
       <c r="L95">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>326406.08738999994</v>
+        <v>24306.55</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B96" s="2" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="E96" s="4">
         <f>F2</f>
@@ -3615,8 +3610,19 @@
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A97" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="B97" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
+      </c>
+      <c r="C97" s="4">
+        <f>F6+F20+F11</f>
+        <v>30101.097999999998</v>
+      </c>
+      <c r="D97" s="4">
+        <f>F10+F22+F12</f>
+        <v>48896.791299999997</v>
       </c>
       <c r="E97" s="4">
         <f>F2</f>
@@ -3624,36 +3630,44 @@
       </c>
       <c r="F97" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>585.70000000000005</v>
+        <v>16385.277859999998</v>
       </c>
       <c r="G97" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>292.85000000000002</v>
+        <v>8192.6389299999992</v>
       </c>
       <c r="H97" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>12592.550000000001</v>
+        <v>194287.69538999998</v>
       </c>
       <c r="I97" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>15521.050000000001</v>
+        <v>227317.29338999998</v>
       </c>
       <c r="J97" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>18449.55</v>
+        <v>260346.89138999998</v>
       </c>
       <c r="K97" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>21378.05</v>
+        <v>293376.48938999994</v>
       </c>
       <c r="L97">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>24306.55</v>
+        <v>326406.08738999994</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B98" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
+      </c>
+      <c r="C98" s="4">
+        <f>F6+F20+F11+F33</f>
+        <v>32293.701999999997</v>
+      </c>
+      <c r="D98" s="4">
+        <f>F10+F22+F12+F33</f>
+        <v>51089.395299999996</v>
       </c>
       <c r="E98" s="4">
         <f>F2</f>
@@ -3661,44 +3675,36 @@
       </c>
       <c r="F98" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>585.70000000000005</v>
+        <v>17262.319459999999</v>
       </c>
       <c r="G98" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>292.85000000000002</v>
+        <v>8631.1597299999994</v>
       </c>
       <c r="H98" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>12592.550000000001</v>
+        <v>204373.67378999997</v>
       </c>
       <c r="I98" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>15521.050000000001</v>
+        <v>239595.87578999996</v>
       </c>
       <c r="J98" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>18449.55</v>
+        <v>274818.07778999995</v>
       </c>
       <c r="K98" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>21378.05</v>
+        <v>310040.27979</v>
       </c>
       <c r="L98">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>24306.55</v>
+        <v>345262.48179000005</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B99" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C99" s="4">
-        <f>F6+F25+F11</f>
-        <v>31335.543900000004</v>
-      </c>
-      <c r="D99" s="4">
-        <f>F10+F27+F12</f>
-        <v>51112.043300000005</v>
+        <v>162</v>
       </c>
       <c r="E99" s="4">
         <f>F2</f>
@@ -3706,36 +3712,36 @@
       </c>
       <c r="F99" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>17075.21744</v>
+        <v>585.70000000000005</v>
       </c>
       <c r="G99" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>8537.6087200000002</v>
+        <v>292.85000000000002</v>
       </c>
       <c r="H99" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>202222.00056000001</v>
+        <v>12592.550000000001</v>
       </c>
       <c r="I99" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>236486.04446</v>
+        <v>15521.050000000001</v>
       </c>
       <c r="J99" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>270750.08836000005</v>
+        <v>18449.55</v>
       </c>
       <c r="K99" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>305014.13226000004</v>
+        <v>21378.05</v>
       </c>
       <c r="L99">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>339278.17616000003</v>
+        <v>24306.55</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B100" s="2" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="E100" s="4">
         <f>F2</f>
@@ -3772,7 +3778,15 @@
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B101" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
+      </c>
+      <c r="C101" s="4">
+        <f>F6+F25+F11</f>
+        <v>31335.543900000004</v>
+      </c>
+      <c r="D101" s="4">
+        <f>F10+F27+F12</f>
+        <v>51112.043300000005</v>
       </c>
       <c r="E101" s="4">
         <f>F2</f>
@@ -3780,36 +3794,44 @@
       </c>
       <c r="F101" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>585.70000000000005</v>
+        <v>17075.21744</v>
       </c>
       <c r="G101" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>292.85000000000002</v>
+        <v>8537.6087200000002</v>
       </c>
       <c r="H101" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>12592.550000000001</v>
+        <v>202222.00056000001</v>
       </c>
       <c r="I101" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>15521.050000000001</v>
+        <v>236486.04446</v>
       </c>
       <c r="J101" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>18449.55</v>
+        <v>270750.08836000005</v>
       </c>
       <c r="K101" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>21378.05</v>
+        <v>305014.13226000004</v>
       </c>
       <c r="L101">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>24306.55</v>
+        <v>339278.17616000003</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B102" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
+      </c>
+      <c r="C102" s="4">
+        <f>F6+F25+F11+F33</f>
+        <v>33528.147900000004</v>
+      </c>
+      <c r="D102" s="4">
+        <f>F10+F27+F12+F33</f>
+        <v>53304.647300000004</v>
       </c>
       <c r="E102" s="4">
         <f>F2</f>
@@ -3817,44 +3839,36 @@
       </c>
       <c r="F102" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>585.70000000000005</v>
+        <v>17952.259040000001</v>
       </c>
       <c r="G102" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>292.85000000000002</v>
+        <v>8976.1295200000004</v>
       </c>
       <c r="H102" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>12592.550000000001</v>
+        <v>212307.97896000001</v>
       </c>
       <c r="I102" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>15521.050000000001</v>
+        <v>248764.62686000002</v>
       </c>
       <c r="J102" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>18449.55</v>
+        <v>285221.27476</v>
       </c>
       <c r="K102" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>21378.05</v>
+        <v>321677.92266000004</v>
       </c>
       <c r="L102">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>24306.55</v>
+        <v>358134.57056000002</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B103" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C103" s="4">
-        <f>F6+F30+F11</f>
-        <v>30631.491600000001</v>
-      </c>
-      <c r="D103" s="4">
-        <f>F10+F32+F12</f>
-        <v>49848.599300000002</v>
+        <v>174</v>
       </c>
       <c r="E103" s="4">
         <f>F2</f>
@@ -3862,36 +3876,36 @@
       </c>
       <c r="F103" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>16681.718180000003</v>
+        <v>585.70000000000005</v>
       </c>
       <c r="G103" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>8340.8590900000017</v>
+        <v>292.85000000000002</v>
       </c>
       <c r="H103" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>197696.75907000003</v>
+        <v>12592.550000000001</v>
       </c>
       <c r="I103" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>231256.75067000001</v>
+        <v>15521.050000000001</v>
       </c>
       <c r="J103" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>264816.74226999999</v>
+        <v>18449.55</v>
       </c>
       <c r="K103" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>298376.73387</v>
+        <v>21378.05</v>
       </c>
       <c r="L103">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>331936.72547</v>
+        <v>24306.55</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B104" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E104" s="4">
         <f>F2</f>
@@ -3928,7 +3942,15 @@
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B105" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
+      </c>
+      <c r="C105" s="4">
+        <f>F6+F30+F11</f>
+        <v>30631.491600000001</v>
+      </c>
+      <c r="D105" s="4">
+        <f>F10+F32+F12</f>
+        <v>49848.599300000002</v>
       </c>
       <c r="E105" s="4">
         <f>F2</f>
@@ -3936,36 +3958,44 @@
       </c>
       <c r="F105" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>585.70000000000005</v>
+        <v>16681.718180000003</v>
       </c>
       <c r="G105" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>292.85000000000002</v>
+        <v>8340.8590900000017</v>
       </c>
       <c r="H105" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>12592.550000000001</v>
+        <v>197696.75907000003</v>
       </c>
       <c r="I105" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>15521.050000000001</v>
+        <v>231256.75067000001</v>
       </c>
       <c r="J105" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>18449.55</v>
+        <v>264816.74226999999</v>
       </c>
       <c r="K105" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>21378.05</v>
+        <v>298376.73387</v>
       </c>
       <c r="L105">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>24306.55</v>
+        <v>331936.72547</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B106" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="C106" s="4">
+        <f>F6+F30+F11+F33</f>
+        <v>32824.095600000001</v>
+      </c>
+      <c r="D106" s="4">
+        <f>F10+F32+F12+F33</f>
+        <v>52041.203300000001</v>
       </c>
       <c r="E106" s="4">
         <f>F2</f>
@@ -3973,47 +4003,36 @@
       </c>
       <c r="F106" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>585.70000000000005</v>
+        <v>17558.75978</v>
       </c>
       <c r="G106" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>292.85000000000002</v>
+        <v>8779.3798900000002</v>
       </c>
       <c r="H106" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>12592.550000000001</v>
+        <v>207782.73746999999</v>
       </c>
       <c r="I106" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>15521.050000000001</v>
+        <v>243535.33306999999</v>
       </c>
       <c r="J106" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>18449.55</v>
+        <v>279287.92866999999</v>
       </c>
       <c r="K106" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>21378.05</v>
+        <v>315040.52426999999</v>
       </c>
       <c r="L106">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>24306.55</v>
+        <v>350793.11986999999</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A107" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="B107" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C107" s="4">
-        <f>F6+F20+F13</f>
-        <v>33202.001199999999</v>
-      </c>
-      <c r="D107" s="4">
-        <f>F10+F22+F14</f>
-        <v>54786.638500000001</v>
+        <v>177</v>
       </c>
       <c r="E107" s="4">
         <f>F2</f>
@@ -4021,36 +4040,36 @@
       </c>
       <c r="F107" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>18183.427940000001</v>
+        <v>585.70000000000005</v>
       </c>
       <c r="G107" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>9091.7139700000007</v>
+        <v>292.85000000000002</v>
       </c>
       <c r="H107" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>214966.42131000001</v>
+        <v>12592.550000000001</v>
       </c>
       <c r="I107" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>251096.92251</v>
+        <v>15521.050000000001</v>
       </c>
       <c r="J107" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>287227.42371</v>
+        <v>18449.55</v>
       </c>
       <c r="K107" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>323357.92491</v>
+        <v>21378.05</v>
       </c>
       <c r="L107">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>359488.42611</v>
+        <v>24306.55</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B108" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E108" s="4">
         <f>F2</f>
@@ -4086,8 +4105,19 @@
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A109" s="2" t="s">
+        <v>180</v>
+      </c>
       <c r="B109" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
+      </c>
+      <c r="C109" s="4">
+        <f>F6+F20+F13</f>
+        <v>33202.001199999999</v>
+      </c>
+      <c r="D109" s="4">
+        <f>F10+F22+F14</f>
+        <v>54786.638500000001</v>
       </c>
       <c r="E109" s="4">
         <f>F2</f>
@@ -4095,36 +4125,44 @@
       </c>
       <c r="F109" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>585.70000000000005</v>
+        <v>18183.427940000001</v>
       </c>
       <c r="G109" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>292.85000000000002</v>
+        <v>9091.7139700000007</v>
       </c>
       <c r="H109" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>12592.550000000001</v>
+        <v>214966.42131000001</v>
       </c>
       <c r="I109" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>15521.050000000001</v>
+        <v>251096.92251</v>
       </c>
       <c r="J109" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>18449.55</v>
+        <v>287227.42371</v>
       </c>
       <c r="K109" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>21378.05</v>
+        <v>323357.92491</v>
       </c>
       <c r="L109">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>24306.55</v>
+        <v>359488.42611</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B110" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
+      </c>
+      <c r="C110" s="4">
+        <f>F6+F20+F13+F33</f>
+        <v>35394.605199999998</v>
+      </c>
+      <c r="D110" s="4">
+        <f>F10+F22+F14+F33</f>
+        <v>56979.2425</v>
       </c>
       <c r="E110" s="4">
         <f>F2</f>
@@ -4132,44 +4170,36 @@
       </c>
       <c r="F110" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>585.70000000000005</v>
+        <v>19060.469539999998</v>
       </c>
       <c r="G110" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>292.85000000000002</v>
+        <v>9530.2347699999991</v>
       </c>
       <c r="H110" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>12592.550000000001</v>
+        <v>225052.39971</v>
       </c>
       <c r="I110" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>15521.050000000001</v>
+        <v>263375.50491000002</v>
       </c>
       <c r="J110" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>18449.55</v>
+        <v>301698.61011000001</v>
       </c>
       <c r="K110" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>21378.05</v>
+        <v>340021.71531</v>
       </c>
       <c r="L110">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>24306.55</v>
+        <v>378344.82050999999</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B111" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C111" s="4">
-        <f>F6+F25+F13</f>
-        <v>34436.447100000005</v>
-      </c>
-      <c r="D111" s="4">
-        <f>F10+F27+F14</f>
-        <v>57001.890500000001</v>
+        <v>183</v>
       </c>
       <c r="E111" s="4">
         <f>F2</f>
@@ -4177,36 +4207,36 @@
       </c>
       <c r="F111" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>18873.36752</v>
+        <v>585.70000000000005</v>
       </c>
       <c r="G111" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>9436.6837599999999</v>
+        <v>292.85000000000002</v>
       </c>
       <c r="H111" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>222900.72648000001</v>
+        <v>12592.550000000001</v>
       </c>
       <c r="I111" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>260265.67358</v>
+        <v>15521.050000000001</v>
       </c>
       <c r="J111" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>297630.62067999999</v>
+        <v>18449.55</v>
       </c>
       <c r="K111" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>334995.56777999998</v>
+        <v>21378.05</v>
       </c>
       <c r="L111">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>372360.51487999997</v>
+        <v>24306.55</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B112" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E112" s="4">
         <f>F2</f>
@@ -4243,7 +4273,15 @@
     </row>
     <row r="113" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B113" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
+      </c>
+      <c r="C113" s="4">
+        <f>F6+F25+F13</f>
+        <v>34436.447100000005</v>
+      </c>
+      <c r="D113" s="4">
+        <f>F10+F27+F14</f>
+        <v>57001.890500000001</v>
       </c>
       <c r="E113" s="4">
         <f>F2</f>
@@ -4251,36 +4289,44 @@
       </c>
       <c r="F113" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>585.70000000000005</v>
+        <v>18873.36752</v>
       </c>
       <c r="G113" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>292.85000000000002</v>
+        <v>9436.6837599999999</v>
       </c>
       <c r="H113" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>12592.550000000001</v>
+        <v>222900.72648000001</v>
       </c>
       <c r="I113" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>15521.050000000001</v>
+        <v>260265.67358</v>
       </c>
       <c r="J113" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>18449.55</v>
+        <v>297630.62067999999</v>
       </c>
       <c r="K113" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>21378.05</v>
+        <v>334995.56777999998</v>
       </c>
       <c r="L113">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>24306.55</v>
+        <v>372360.51487999997</v>
       </c>
     </row>
     <row r="114" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B114" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
+      </c>
+      <c r="C114" s="4">
+        <f>F6+F25+F13+F33</f>
+        <v>36629.051100000004</v>
+      </c>
+      <c r="D114" s="4">
+        <f>F10+F27+F14+F33</f>
+        <v>59194.494500000001</v>
       </c>
       <c r="E114" s="4">
         <f>F2</f>
@@ -4288,44 +4334,36 @@
       </c>
       <c r="F114" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>585.70000000000005</v>
+        <v>19750.409120000004</v>
       </c>
       <c r="G114" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>292.85000000000002</v>
+        <v>9875.2045600000019</v>
       </c>
       <c r="H114" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>12592.550000000001</v>
+        <v>232986.70488000003</v>
       </c>
       <c r="I114" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>15521.050000000001</v>
+        <v>272544.25598000002</v>
       </c>
       <c r="J114" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>18449.55</v>
+        <v>312101.80708</v>
       </c>
       <c r="K114" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>21378.05</v>
+        <v>351659.35818000004</v>
       </c>
       <c r="L114">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>24306.55</v>
+        <v>391216.90928000002</v>
       </c>
     </row>
     <row r="115" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B115" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C115" s="4">
-        <f>F6+F30+F13</f>
-        <v>33732.394800000002</v>
-      </c>
-      <c r="D115" s="4">
-        <f>F10+F32+F14</f>
-        <v>55738.446500000005</v>
+        <v>187</v>
       </c>
       <c r="E115" s="4">
         <f>F2</f>
@@ -4333,36 +4371,36 @@
       </c>
       <c r="F115" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>18479.868259999999</v>
+        <v>585.70000000000005</v>
       </c>
       <c r="G115" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>9239.9341299999996</v>
+        <v>292.85000000000002</v>
       </c>
       <c r="H115" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>218375.48499</v>
+        <v>12592.550000000001</v>
       </c>
       <c r="I115" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>255036.37979000001</v>
+        <v>15521.050000000001</v>
       </c>
       <c r="J115" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>291697.27459000004</v>
+        <v>18449.55</v>
       </c>
       <c r="K115" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>328358.16939000005</v>
+        <v>21378.05</v>
       </c>
       <c r="L115">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>365019.06419</v>
+        <v>24306.55</v>
       </c>
     </row>
     <row r="116" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B116" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E116" s="4">
         <f>F2</f>
@@ -4399,7 +4437,15 @@
     </row>
     <row r="117" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B117" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
+      </c>
+      <c r="C117" s="4">
+        <f>F6+F30+F13</f>
+        <v>33732.394800000002</v>
+      </c>
+      <c r="D117" s="4">
+        <f>F10+F32+F14</f>
+        <v>55738.446500000005</v>
       </c>
       <c r="E117" s="4">
         <f>F2</f>
@@ -4407,36 +4453,44 @@
       </c>
       <c r="F117" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>585.70000000000005</v>
+        <v>18479.868259999999</v>
       </c>
       <c r="G117" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>292.85000000000002</v>
+        <v>9239.9341299999996</v>
       </c>
       <c r="H117" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>12592.550000000001</v>
+        <v>218375.48499</v>
       </c>
       <c r="I117" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>15521.050000000001</v>
+        <v>255036.37979000001</v>
       </c>
       <c r="J117" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>18449.55</v>
+        <v>291697.27459000004</v>
       </c>
       <c r="K117" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>21378.05</v>
+        <v>328358.16939000005</v>
       </c>
       <c r="L117">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>24306.55</v>
+        <v>365019.06419</v>
       </c>
     </row>
     <row r="118" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B118" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
+      </c>
+      <c r="C118" s="4">
+        <f>F6+F30+F13+F33</f>
+        <v>35924.998800000001</v>
+      </c>
+      <c r="D118" s="4">
+        <f>F10+F32+F14+F33</f>
+        <v>57931.050500000005</v>
       </c>
       <c r="E118" s="4">
         <f>F2</f>
@@ -4444,29 +4498,103 @@
       </c>
       <c r="F118" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
-        <v>585.70000000000005</v>
+        <v>19356.909860000003</v>
       </c>
       <c r="G118" s="4">
         <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
-        <v>292.85000000000002</v>
+        <v>9678.4549300000017</v>
       </c>
       <c r="H118" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>12592.550000000001</v>
+        <v>228461.46339000005</v>
       </c>
       <c r="I118" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>15521.050000000001</v>
+        <v>267314.96219000005</v>
       </c>
       <c r="J118" s="4">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
-        <v>18449.55</v>
+        <v>306168.46099000005</v>
       </c>
       <c r="K118" s="1">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
+        <v>345021.95979000005</v>
+      </c>
+      <c r="L118">
+        <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
+        <v>383875.45859000005</v>
+      </c>
+    </row>
+    <row r="119" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B119" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E119" s="4">
+        <f>F2</f>
+        <v>2928.5</v>
+      </c>
+      <c r="F119" s="4">
+        <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
+        <v>585.70000000000005</v>
+      </c>
+      <c r="G119" s="4">
+        <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
+        <v>292.85000000000002</v>
+      </c>
+      <c r="H119" s="4">
+        <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
+        <v>12592.550000000001</v>
+      </c>
+      <c r="I119" s="4">
+        <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
+        <v>15521.050000000001</v>
+      </c>
+      <c r="J119" s="4">
+        <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
+        <v>18449.55</v>
+      </c>
+      <c r="K119" s="1">
+        <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
         <v>21378.05</v>
       </c>
-      <c r="L118">
+      <c r="L119">
+        <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
+        <v>24306.55</v>
+      </c>
+    </row>
+    <row r="120" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B120" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E120" s="4">
+        <f>F2</f>
+        <v>2928.5</v>
+      </c>
+      <c r="F120" s="4">
+        <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*20/100</f>
+        <v>585.70000000000005</v>
+      </c>
+      <c r="G120" s="4">
+        <f>(Tabelle2[[#This Row],[Mittelmodul]]+Tabelle2[[#This Row],[Abschlussmodul]]+Tabelle2[[#This Row],[Zusatzkosten/Modul]])*10/100</f>
+        <v>292.85000000000002</v>
+      </c>
+      <c r="H120" s="4">
+        <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(2*Tabelle2[[#This Row],[Mittelmodul]])+(4*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
+        <v>12592.550000000001</v>
+      </c>
+      <c r="I120" s="4">
+        <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(3*Tabelle2[[#This Row],[Mittelmodul]])+(5*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
+        <v>15521.050000000001</v>
+      </c>
+      <c r="J120" s="4">
+        <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(4*Tabelle2[[#This Row],[Mittelmodul]])+(6*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
+        <v>18449.55</v>
+      </c>
+      <c r="K120" s="1">
+        <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(5*Tabelle2[[#This Row],[Mittelmodul]])+(7*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
+        <v>21378.05</v>
+      </c>
+      <c r="L120">
         <f>(2*Tabelle2[[#This Row],[Abschlussmodul]])+(6*Tabelle2[[#This Row],[Mittelmodul]])+(8*Tabelle2[[#This Row],[Zusatzkosten/Modul]])+Tabelle2[[#This Row],[UST 20%]]+Tabelle2[[#This Row],[Zuschlag Gew.]]</f>
         <v>24306.55</v>
       </c>

</xml_diff>